<commit_message>
Adiciondo tudin2 a o git
</commit_message>
<xml_diff>
--- a/tudin2.xlsx
+++ b/tudin2.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Desktop\pacman_assembly_mips\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{644586B7-572F-47AF-B957-1D4ABFA2C33B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -19,8 +13,8 @@
     <sheet name="Planilha4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,8 +22,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -40,6 +34,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -487,7 +487,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -542,10 +542,14 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -606,7 +610,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -658,7 +662,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -852,21 +856,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:DX64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AP16" sqref="AP16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="AK31" sqref="AK31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.140625" customWidth="1"/>
@@ -885,7 +889,7 @@
     <col min="24" max="31" width="6.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:128">
       <c r="A1" s="16">
         <v>0</v>
       </c>
@@ -1206,7 +1210,7 @@
       <c r="DW1" s="1"/>
       <c r="DX1" s="1"/>
     </row>
-    <row r="2" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:128">
       <c r="A2" s="16">
         <f t="shared" ref="A2:AE2" si="2">A1+256</f>
         <v>256</v>
@@ -1347,7 +1351,7 @@
         <f t="shared" si="3"/>
         <v>392</v>
       </c>
-      <c r="AJ2" s="54">
+      <c r="AJ2" s="57">
         <f t="shared" si="3"/>
         <v>396</v>
       </c>
@@ -1528,7 +1532,7 @@
       <c r="DW2" s="1"/>
       <c r="DX2" s="1"/>
     </row>
-    <row r="3" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:128">
       <c r="A3" s="16">
         <f t="shared" ref="A3:A32" si="4">A2+256</f>
         <v>512</v>
@@ -1669,7 +1673,7 @@
         <f t="shared" ref="AI3:AI32" si="38">AI2+256</f>
         <v>648</v>
       </c>
-      <c r="AJ3" s="55">
+      <c r="AJ3" s="58">
         <f t="shared" ref="AJ3:AJ32" si="39">AJ2+256</f>
         <v>652</v>
       </c>
@@ -1689,7 +1693,7 @@
         <f t="shared" ref="AN3:AN32" si="43">AN2+256</f>
         <v>668</v>
       </c>
-      <c r="AO3" s="55">
+      <c r="AO3" s="58">
         <f t="shared" ref="AO3:AO32" si="44">AO2+256</f>
         <v>672</v>
       </c>
@@ -1713,7 +1717,7 @@
         <f t="shared" ref="AT3:AT32" si="49">AT2+256</f>
         <v>692</v>
       </c>
-      <c r="AU3" s="55">
+      <c r="AU3" s="58">
         <f t="shared" ref="AU3:AU32" si="50">AU2+256</f>
         <v>696</v>
       </c>
@@ -1721,7 +1725,7 @@
         <f t="shared" ref="AV3:AV32" si="51">AV2+256</f>
         <v>700</v>
       </c>
-      <c r="AW3" s="55">
+      <c r="AW3" s="58">
         <f t="shared" ref="AW3:AW32" si="52">AW2+256</f>
         <v>704</v>
       </c>
@@ -1749,11 +1753,11 @@
         <f t="shared" ref="BC3:BC32" si="58">BC2+256</f>
         <v>728</v>
       </c>
-      <c r="BD3" s="55">
+      <c r="BD3" s="58">
         <f t="shared" ref="BD3:BD32" si="59">BD2+256</f>
         <v>732</v>
       </c>
-      <c r="BE3" s="55">
+      <c r="BE3" s="58">
         <f t="shared" ref="BE3:BE32" si="60">BE2+256</f>
         <v>736</v>
       </c>
@@ -1777,11 +1781,11 @@
         <f t="shared" ref="BJ3:BJ32" si="65">BJ2+256</f>
         <v>756</v>
       </c>
-      <c r="BK3" s="55">
+      <c r="BK3" s="54">
         <f t="shared" ref="BK3:BK32" si="66">BK2+256</f>
         <v>760</v>
       </c>
-      <c r="BL3" s="56">
+      <c r="BL3" s="55">
         <f t="shared" ref="BL3:BL32" si="67">BL2+256</f>
         <v>764</v>
       </c>
@@ -1850,7 +1854,7 @@
       <c r="DW3" s="1"/>
       <c r="DX3" s="1"/>
     </row>
-    <row r="4" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:128">
       <c r="A4" s="16">
         <f t="shared" si="4"/>
         <v>768</v>
@@ -1991,7 +1995,7 @@
         <f t="shared" si="38"/>
         <v>904</v>
       </c>
-      <c r="AJ4" s="55">
+      <c r="AJ4" s="58">
         <f t="shared" si="39"/>
         <v>908</v>
       </c>
@@ -2011,7 +2015,7 @@
         <f t="shared" si="43"/>
         <v>924</v>
       </c>
-      <c r="AO4" s="55">
+      <c r="AO4" s="58">
         <f t="shared" si="44"/>
         <v>928</v>
       </c>
@@ -2035,7 +2039,7 @@
         <f t="shared" si="49"/>
         <v>948</v>
       </c>
-      <c r="AU4" s="55">
+      <c r="AU4" s="58">
         <f t="shared" si="50"/>
         <v>952</v>
       </c>
@@ -2043,7 +2047,7 @@
         <f t="shared" si="51"/>
         <v>956</v>
       </c>
-      <c r="AW4" s="55">
+      <c r="AW4" s="58">
         <f t="shared" si="52"/>
         <v>960</v>
       </c>
@@ -2071,11 +2075,11 @@
         <f t="shared" si="58"/>
         <v>984</v>
       </c>
-      <c r="BD4" s="55">
+      <c r="BD4" s="58">
         <f t="shared" si="59"/>
         <v>988</v>
       </c>
-      <c r="BE4" s="55">
+      <c r="BE4" s="58">
         <f t="shared" si="60"/>
         <v>992</v>
       </c>
@@ -2099,11 +2103,11 @@
         <f t="shared" si="65"/>
         <v>1012</v>
       </c>
-      <c r="BK4" s="55">
+      <c r="BK4" s="54">
         <f t="shared" si="66"/>
         <v>1016</v>
       </c>
-      <c r="BL4" s="56">
+      <c r="BL4" s="55">
         <f t="shared" si="67"/>
         <v>1020</v>
       </c>
@@ -2172,7 +2176,7 @@
       <c r="DW4" s="1"/>
       <c r="DX4" s="1"/>
     </row>
-    <row r="5" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:128">
       <c r="A5" s="16">
         <f t="shared" si="4"/>
         <v>1024</v>
@@ -2313,7 +2317,7 @@
         <f t="shared" si="38"/>
         <v>1160</v>
       </c>
-      <c r="AJ5" s="55">
+      <c r="AJ5" s="58">
         <f t="shared" si="39"/>
         <v>1164</v>
       </c>
@@ -2333,7 +2337,7 @@
         <f t="shared" si="43"/>
         <v>1180</v>
       </c>
-      <c r="AO5" s="55">
+      <c r="AO5" s="58">
         <f t="shared" si="44"/>
         <v>1184</v>
       </c>
@@ -2357,7 +2361,7 @@
         <f t="shared" si="49"/>
         <v>1204</v>
       </c>
-      <c r="AU5" s="55">
+      <c r="AU5" s="58">
         <f t="shared" si="50"/>
         <v>1208</v>
       </c>
@@ -2365,7 +2369,7 @@
         <f t="shared" si="51"/>
         <v>1212</v>
       </c>
-      <c r="AW5" s="55">
+      <c r="AW5" s="58">
         <f t="shared" si="52"/>
         <v>1216</v>
       </c>
@@ -2389,7 +2393,7 @@
         <f t="shared" si="57"/>
         <v>1236</v>
       </c>
-      <c r="BC5" s="55">
+      <c r="BC5" s="58">
         <f t="shared" si="58"/>
         <v>1240</v>
       </c>
@@ -2397,7 +2401,7 @@
         <f t="shared" si="59"/>
         <v>1244</v>
       </c>
-      <c r="BE5" s="55">
+      <c r="BE5" s="58">
         <f t="shared" si="60"/>
         <v>1248</v>
       </c>
@@ -2494,7 +2498,7 @@
       <c r="DW5" s="1"/>
       <c r="DX5" s="1"/>
     </row>
-    <row r="6" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:128">
       <c r="A6" s="16">
         <f t="shared" si="4"/>
         <v>1280</v>
@@ -2635,7 +2639,7 @@
         <f t="shared" si="38"/>
         <v>1416</v>
       </c>
-      <c r="AJ6" s="55">
+      <c r="AJ6" s="58">
         <f t="shared" si="39"/>
         <v>1420</v>
       </c>
@@ -2655,7 +2659,7 @@
         <f t="shared" si="43"/>
         <v>1436</v>
       </c>
-      <c r="AO6" s="55">
+      <c r="AO6" s="58">
         <f t="shared" si="44"/>
         <v>1440</v>
       </c>
@@ -2679,7 +2683,7 @@
         <f t="shared" si="49"/>
         <v>1460</v>
       </c>
-      <c r="AU6" s="55">
+      <c r="AU6" s="58">
         <f t="shared" si="50"/>
         <v>1464</v>
       </c>
@@ -2687,7 +2691,7 @@
         <f t="shared" si="51"/>
         <v>1468</v>
       </c>
-      <c r="AW6" s="55">
+      <c r="AW6" s="58">
         <f t="shared" si="52"/>
         <v>1472</v>
       </c>
@@ -2711,7 +2715,7 @@
         <f t="shared" si="57"/>
         <v>1492</v>
       </c>
-      <c r="BC6" s="55">
+      <c r="BC6" s="58">
         <f t="shared" si="58"/>
         <v>1496</v>
       </c>
@@ -2719,7 +2723,7 @@
         <f t="shared" si="59"/>
         <v>1500</v>
       </c>
-      <c r="BE6" s="55">
+      <c r="BE6" s="58">
         <f t="shared" si="60"/>
         <v>1504</v>
       </c>
@@ -2743,11 +2747,11 @@
         <f t="shared" si="65"/>
         <v>1524</v>
       </c>
-      <c r="BK6" s="55">
+      <c r="BK6" s="54">
         <f t="shared" si="66"/>
         <v>1528</v>
       </c>
-      <c r="BL6" s="56">
+      <c r="BL6" s="55">
         <f t="shared" si="67"/>
         <v>1532</v>
       </c>
@@ -2816,7 +2820,7 @@
       <c r="DW6" s="1"/>
       <c r="DX6" s="1"/>
     </row>
-    <row r="7" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:128">
       <c r="A7" s="16">
         <f t="shared" si="4"/>
         <v>1536</v>
@@ -2957,7 +2961,7 @@
         <f t="shared" si="38"/>
         <v>1672</v>
       </c>
-      <c r="AJ7" s="55">
+      <c r="AJ7" s="58">
         <f t="shared" si="39"/>
         <v>1676</v>
       </c>
@@ -2981,7 +2985,7 @@
         <f t="shared" si="44"/>
         <v>1696</v>
       </c>
-      <c r="AP7" s="55">
+      <c r="AP7" s="58">
         <f t="shared" si="45"/>
         <v>1700</v>
       </c>
@@ -2997,7 +3001,7 @@
         <f t="shared" si="48"/>
         <v>1712</v>
       </c>
-      <c r="AT7" s="55">
+      <c r="AT7" s="58">
         <f t="shared" si="49"/>
         <v>1716</v>
       </c>
@@ -3009,7 +3013,7 @@
         <f t="shared" si="51"/>
         <v>1724</v>
       </c>
-      <c r="AW7" s="55">
+      <c r="AW7" s="58">
         <f t="shared" si="52"/>
         <v>1728</v>
       </c>
@@ -3041,7 +3045,7 @@
         <f t="shared" si="59"/>
         <v>1756</v>
       </c>
-      <c r="BE7" s="55">
+      <c r="BE7" s="58">
         <f t="shared" si="60"/>
         <v>1760</v>
       </c>
@@ -3065,11 +3069,11 @@
         <f t="shared" si="65"/>
         <v>1780</v>
       </c>
-      <c r="BK7" s="55">
+      <c r="BK7" s="54">
         <f t="shared" si="66"/>
         <v>1784</v>
       </c>
-      <c r="BL7" s="56">
+      <c r="BL7" s="55">
         <f t="shared" si="67"/>
         <v>1788</v>
       </c>
@@ -3138,7 +3142,7 @@
       <c r="DW7" s="1"/>
       <c r="DX7" s="1"/>
     </row>
-    <row r="8" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:128">
       <c r="A8" s="16">
         <f t="shared" si="4"/>
         <v>1792</v>
@@ -3279,7 +3283,7 @@
         <f t="shared" si="38"/>
         <v>1928</v>
       </c>
-      <c r="AJ8" s="55">
+      <c r="AJ8" s="58">
         <f t="shared" si="39"/>
         <v>1932</v>
       </c>
@@ -3303,7 +3307,7 @@
         <f t="shared" si="44"/>
         <v>1952</v>
       </c>
-      <c r="AP8" s="55">
+      <c r="AP8" s="58">
         <f t="shared" si="45"/>
         <v>1956</v>
       </c>
@@ -3319,7 +3323,7 @@
         <f t="shared" si="48"/>
         <v>1968</v>
       </c>
-      <c r="AT8" s="55">
+      <c r="AT8" s="58">
         <f t="shared" si="49"/>
         <v>1972</v>
       </c>
@@ -3331,7 +3335,7 @@
         <f t="shared" si="51"/>
         <v>1980</v>
       </c>
-      <c r="AW8" s="55">
+      <c r="AW8" s="58">
         <f t="shared" si="52"/>
         <v>1984</v>
       </c>
@@ -3363,7 +3367,7 @@
         <f t="shared" si="59"/>
         <v>2012</v>
       </c>
-      <c r="BE8" s="55">
+      <c r="BE8" s="58">
         <f t="shared" si="60"/>
         <v>2016</v>
       </c>
@@ -3460,7 +3464,7 @@
       <c r="DW8" s="1"/>
       <c r="DX8" s="1"/>
     </row>
-    <row r="9" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:128">
       <c r="A9" s="16">
         <f t="shared" si="4"/>
         <v>2048</v>
@@ -3601,7 +3605,7 @@
         <f t="shared" si="38"/>
         <v>2184</v>
       </c>
-      <c r="AJ9" s="55">
+      <c r="AJ9" s="58">
         <f t="shared" si="39"/>
         <v>2188</v>
       </c>
@@ -3625,7 +3629,7 @@
         <f t="shared" si="44"/>
         <v>2208</v>
       </c>
-      <c r="AP9" s="55">
+      <c r="AP9" s="58">
         <f t="shared" si="45"/>
         <v>2212</v>
       </c>
@@ -3641,7 +3645,7 @@
         <f t="shared" si="48"/>
         <v>2224</v>
       </c>
-      <c r="AT9" s="55">
+      <c r="AT9" s="58">
         <f t="shared" si="49"/>
         <v>2228</v>
       </c>
@@ -3653,7 +3657,7 @@
         <f t="shared" si="51"/>
         <v>2236</v>
       </c>
-      <c r="AW9" s="55">
+      <c r="AW9" s="58">
         <f t="shared" si="52"/>
         <v>2240</v>
       </c>
@@ -3685,7 +3689,7 @@
         <f t="shared" si="59"/>
         <v>2268</v>
       </c>
-      <c r="BE9" s="55">
+      <c r="BE9" s="58">
         <f t="shared" si="60"/>
         <v>2272</v>
       </c>
@@ -3709,10 +3713,10 @@
         <f t="shared" si="65"/>
         <v>2292</v>
       </c>
-      <c r="BK9" s="55">
+      <c r="BK9" s="54">
         <v>65</v>
       </c>
-      <c r="BL9" s="56">
+      <c r="BL9" s="55">
         <f t="shared" si="67"/>
         <v>2300</v>
       </c>
@@ -3781,7 +3785,7 @@
       <c r="DW9" s="1"/>
       <c r="DX9" s="1"/>
     </row>
-    <row r="10" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:128">
       <c r="A10" s="16">
         <f t="shared" si="4"/>
         <v>2304</v>
@@ -3922,7 +3926,7 @@
         <f t="shared" si="38"/>
         <v>2440</v>
       </c>
-      <c r="AJ10" s="55">
+      <c r="AJ10" s="58">
         <f t="shared" si="39"/>
         <v>2444</v>
       </c>
@@ -3950,7 +3954,7 @@
         <f t="shared" si="45"/>
         <v>2468</v>
       </c>
-      <c r="AQ10" s="55">
+      <c r="AQ10" s="58">
         <f t="shared" si="46"/>
         <v>2472</v>
       </c>
@@ -3958,7 +3962,7 @@
         <f t="shared" si="47"/>
         <v>2476</v>
       </c>
-      <c r="AS10" s="55">
+      <c r="AS10" s="58">
         <f t="shared" si="48"/>
         <v>2480</v>
       </c>
@@ -3974,7 +3978,7 @@
         <f t="shared" si="51"/>
         <v>2492</v>
       </c>
-      <c r="AW10" s="55">
+      <c r="AW10" s="58">
         <f t="shared" si="52"/>
         <v>2496</v>
       </c>
@@ -4006,7 +4010,7 @@
         <f t="shared" si="59"/>
         <v>2524</v>
       </c>
-      <c r="BE10" s="55">
+      <c r="BE10" s="58">
         <f t="shared" si="60"/>
         <v>2528</v>
       </c>
@@ -4030,11 +4034,11 @@
         <f t="shared" si="65"/>
         <v>2548</v>
       </c>
-      <c r="BK10" s="55">
+      <c r="BK10" s="54">
         <f t="shared" si="66"/>
         <v>321</v>
       </c>
-      <c r="BL10" s="56">
+      <c r="BL10" s="55">
         <f t="shared" si="67"/>
         <v>2556</v>
       </c>
@@ -4103,7 +4107,7 @@
       <c r="DW10" s="1"/>
       <c r="DX10" s="1"/>
     </row>
-    <row r="11" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:128">
       <c r="A11" s="16">
         <f t="shared" si="4"/>
         <v>2560</v>
@@ -4244,7 +4248,7 @@
         <f t="shared" si="38"/>
         <v>2696</v>
       </c>
-      <c r="AJ11" s="55">
+      <c r="AJ11" s="58">
         <f t="shared" si="39"/>
         <v>2700</v>
       </c>
@@ -4272,7 +4276,7 @@
         <f t="shared" si="45"/>
         <v>2724</v>
       </c>
-      <c r="AQ11" s="55">
+      <c r="AQ11" s="58">
         <f t="shared" si="46"/>
         <v>2728</v>
       </c>
@@ -4280,7 +4284,7 @@
         <f t="shared" si="47"/>
         <v>2732</v>
       </c>
-      <c r="AS11" s="55">
+      <c r="AS11" s="58">
         <f t="shared" si="48"/>
         <v>2736</v>
       </c>
@@ -4296,7 +4300,7 @@
         <f t="shared" si="51"/>
         <v>2748</v>
       </c>
-      <c r="AW11" s="55">
+      <c r="AW11" s="58">
         <f t="shared" si="52"/>
         <v>2752</v>
       </c>
@@ -4328,7 +4332,7 @@
         <f t="shared" si="59"/>
         <v>2780</v>
       </c>
-      <c r="BE11" s="55">
+      <c r="BE11" s="58">
         <f t="shared" si="60"/>
         <v>2784</v>
       </c>
@@ -4425,7 +4429,7 @@
       <c r="DW11" s="1"/>
       <c r="DX11" s="1"/>
     </row>
-    <row r="12" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:128">
       <c r="A12" s="16">
         <f t="shared" si="4"/>
         <v>2816</v>
@@ -4566,19 +4570,19 @@
         <f t="shared" si="38"/>
         <v>2952</v>
       </c>
-      <c r="AJ12" s="55">
+      <c r="AJ12" s="58">
         <f t="shared" si="39"/>
         <v>2956</v>
       </c>
-      <c r="AK12" s="55">
+      <c r="AK12" s="58">
         <f t="shared" si="40"/>
         <v>2960</v>
       </c>
-      <c r="AL12" s="55">
+      <c r="AL12" s="58">
         <f t="shared" si="41"/>
         <v>2964</v>
       </c>
-      <c r="AM12" s="55">
+      <c r="AM12" s="58">
         <f t="shared" si="42"/>
         <v>2968</v>
       </c>
@@ -4598,7 +4602,7 @@
         <f t="shared" si="46"/>
         <v>2984</v>
       </c>
-      <c r="AR12" s="55">
+      <c r="AR12" s="58">
         <f t="shared" si="47"/>
         <v>2988</v>
       </c>
@@ -4618,19 +4622,19 @@
         <f t="shared" si="51"/>
         <v>3004</v>
       </c>
-      <c r="AW12" s="55">
+      <c r="AW12" s="58">
         <f t="shared" si="52"/>
         <v>3008</v>
       </c>
-      <c r="AX12" s="55">
+      <c r="AX12" s="58">
         <f t="shared" si="53"/>
         <v>3012</v>
       </c>
-      <c r="AY12" s="55">
+      <c r="AY12" s="58">
         <f t="shared" si="54"/>
         <v>3016</v>
       </c>
-      <c r="AZ12" s="55">
+      <c r="AZ12" s="58">
         <f t="shared" si="55"/>
         <v>3020</v>
       </c>
@@ -4638,7 +4642,7 @@
         <f t="shared" si="56"/>
         <v>3024</v>
       </c>
-      <c r="BB12" s="55">
+      <c r="BB12" s="54">
         <f t="shared" si="57"/>
         <v>3028</v>
       </c>
@@ -4650,7 +4654,7 @@
         <f t="shared" si="59"/>
         <v>3036</v>
       </c>
-      <c r="BE12" s="55">
+      <c r="BE12" s="58">
         <f t="shared" si="60"/>
         <v>3040</v>
       </c>
@@ -4747,7 +4751,7 @@
       <c r="DW12" s="1"/>
       <c r="DX12" s="1"/>
     </row>
-    <row r="13" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:128">
       <c r="A13" s="16">
         <f t="shared" si="4"/>
         <v>3072</v>
@@ -4888,19 +4892,19 @@
         <f t="shared" si="38"/>
         <v>3208</v>
       </c>
-      <c r="AJ13" s="55">
+      <c r="AJ13" s="58">
         <f t="shared" si="39"/>
         <v>3212</v>
       </c>
-      <c r="AK13" s="55">
+      <c r="AK13" s="58">
         <f t="shared" si="40"/>
         <v>3216</v>
       </c>
-      <c r="AL13" s="55">
+      <c r="AL13" s="58">
         <f t="shared" si="41"/>
         <v>3220</v>
       </c>
-      <c r="AM13" s="55">
+      <c r="AM13" s="58">
         <f t="shared" si="42"/>
         <v>3224</v>
       </c>
@@ -4920,7 +4924,7 @@
         <f t="shared" si="46"/>
         <v>3240</v>
       </c>
-      <c r="AR13" s="55">
+      <c r="AR13" s="58">
         <f t="shared" si="47"/>
         <v>3244</v>
       </c>
@@ -4940,19 +4944,19 @@
         <f t="shared" si="51"/>
         <v>3260</v>
       </c>
-      <c r="AW13" s="55">
+      <c r="AW13" s="58">
         <f t="shared" si="52"/>
         <v>3264</v>
       </c>
-      <c r="AX13" s="55">
+      <c r="AX13" s="58">
         <f t="shared" si="53"/>
         <v>3268</v>
       </c>
-      <c r="AY13" s="55">
+      <c r="AY13" s="58">
         <f t="shared" si="54"/>
         <v>3272</v>
       </c>
-      <c r="AZ13" s="55">
+      <c r="AZ13" s="58">
         <f t="shared" si="55"/>
         <v>3276</v>
       </c>
@@ -4960,7 +4964,7 @@
         <f t="shared" si="56"/>
         <v>3280</v>
       </c>
-      <c r="BB13" s="55">
+      <c r="BB13" s="54">
         <f t="shared" si="57"/>
         <v>3284</v>
       </c>
@@ -4972,7 +4976,7 @@
         <f t="shared" si="59"/>
         <v>3292</v>
       </c>
-      <c r="BE13" s="55">
+      <c r="BE13" s="58">
         <f t="shared" si="60"/>
         <v>3296</v>
       </c>
@@ -5069,7 +5073,7 @@
       <c r="DW13" s="1"/>
       <c r="DX13" s="1"/>
     </row>
-    <row r="14" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:128">
       <c r="A14" s="16">
         <f t="shared" si="4"/>
         <v>3328</v>
@@ -5391,7 +5395,7 @@
       <c r="DW14" s="1"/>
       <c r="DX14" s="1"/>
     </row>
-    <row r="15" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:128">
       <c r="A15" s="16">
         <f t="shared" si="4"/>
         <v>3584</v>
@@ -5713,7 +5717,7 @@
       <c r="DW15" s="1"/>
       <c r="DX15" s="1"/>
     </row>
-    <row r="16" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:128">
       <c r="A16" s="16">
         <f t="shared" si="4"/>
         <v>3840</v>
@@ -5854,19 +5858,19 @@
         <f t="shared" si="38"/>
         <v>3976</v>
       </c>
-      <c r="AJ16" s="55">
+      <c r="AJ16" s="54">
         <f t="shared" si="39"/>
         <v>3980</v>
       </c>
-      <c r="AK16" s="55">
+      <c r="AK16" s="54">
         <f t="shared" si="40"/>
         <v>3984</v>
       </c>
-      <c r="AL16" s="55">
+      <c r="AL16" s="54">
         <f t="shared" si="41"/>
         <v>3988</v>
       </c>
-      <c r="AM16" s="55">
+      <c r="AM16" s="54">
         <f t="shared" si="42"/>
         <v>3992</v>
       </c>
@@ -5882,15 +5886,15 @@
         <f t="shared" si="45"/>
         <v>4004</v>
       </c>
-      <c r="AQ16" s="55">
+      <c r="AQ16" s="54">
         <f t="shared" si="46"/>
         <v>4008</v>
       </c>
-      <c r="AR16" s="55">
+      <c r="AR16" s="54">
         <f t="shared" si="47"/>
         <v>4012</v>
       </c>
-      <c r="AS16" s="55">
+      <c r="AS16" s="54">
         <f t="shared" si="48"/>
         <v>4016</v>
       </c>
@@ -5918,19 +5922,19 @@
         <f t="shared" si="54"/>
         <v>4040</v>
       </c>
-      <c r="AZ16" s="55">
+      <c r="AZ16" s="54">
         <f t="shared" si="55"/>
         <v>4044</v>
       </c>
-      <c r="BA16" s="55">
+      <c r="BA16" s="54">
         <f t="shared" si="56"/>
         <v>4048</v>
       </c>
-      <c r="BB16" s="55">
+      <c r="BB16" s="54">
         <f t="shared" si="57"/>
         <v>4052</v>
       </c>
-      <c r="BC16" s="55">
+      <c r="BC16" s="54">
         <f t="shared" si="58"/>
         <v>4056</v>
       </c>
@@ -6035,7 +6039,7 @@
       <c r="DW16" s="1"/>
       <c r="DX16" s="1"/>
     </row>
-    <row r="17" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:128">
       <c r="A17" s="16">
         <f t="shared" si="4"/>
         <v>4096</v>
@@ -6176,7 +6180,7 @@
         <f t="shared" si="38"/>
         <v>4232</v>
       </c>
-      <c r="AJ17" s="55">
+      <c r="AJ17" s="54">
         <f t="shared" si="39"/>
         <v>4236</v>
       </c>
@@ -6188,7 +6192,7 @@
         <f t="shared" si="41"/>
         <v>4244</v>
       </c>
-      <c r="AM17" s="55">
+      <c r="AM17" s="54">
         <f t="shared" si="42"/>
         <v>4248</v>
       </c>
@@ -6200,7 +6204,7 @@
         <f t="shared" si="44"/>
         <v>4256</v>
       </c>
-      <c r="AP17" s="55">
+      <c r="AP17" s="54">
         <f t="shared" si="45"/>
         <v>4260</v>
       </c>
@@ -6216,7 +6220,7 @@
         <f t="shared" si="48"/>
         <v>4272</v>
       </c>
-      <c r="AT17" s="55">
+      <c r="AT17" s="54">
         <f t="shared" si="49"/>
         <v>4276</v>
       </c>
@@ -6240,7 +6244,7 @@
         <f t="shared" si="54"/>
         <v>4296</v>
       </c>
-      <c r="AZ17" s="55">
+      <c r="AZ17" s="54">
         <f t="shared" si="55"/>
         <v>4300</v>
       </c>
@@ -6252,7 +6256,7 @@
         <f t="shared" si="57"/>
         <v>4308</v>
       </c>
-      <c r="BC17" s="55">
+      <c r="BC17" s="54">
         <f t="shared" si="58"/>
         <v>4312</v>
       </c>
@@ -6357,7 +6361,7 @@
       <c r="DW17" s="1"/>
       <c r="DX17" s="1"/>
     </row>
-    <row r="18" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:128">
       <c r="A18" s="16">
         <f t="shared" si="4"/>
         <v>4352</v>
@@ -6498,7 +6502,7 @@
         <f t="shared" si="38"/>
         <v>4488</v>
       </c>
-      <c r="AJ18" s="55">
+      <c r="AJ18" s="54">
         <f t="shared" si="39"/>
         <v>4492</v>
       </c>
@@ -6510,7 +6514,7 @@
         <f t="shared" si="41"/>
         <v>4500</v>
       </c>
-      <c r="AM18" s="55">
+      <c r="AM18" s="54">
         <f t="shared" si="42"/>
         <v>4504</v>
       </c>
@@ -6522,7 +6526,7 @@
         <f t="shared" si="44"/>
         <v>4512</v>
       </c>
-      <c r="AP18" s="55">
+      <c r="AP18" s="54">
         <f t="shared" si="45"/>
         <v>4516</v>
       </c>
@@ -6538,7 +6542,7 @@
         <f t="shared" si="48"/>
         <v>4528</v>
       </c>
-      <c r="AT18" s="55">
+      <c r="AT18" s="54">
         <f t="shared" si="49"/>
         <v>4532</v>
       </c>
@@ -6562,7 +6566,7 @@
         <f t="shared" si="54"/>
         <v>4552</v>
       </c>
-      <c r="AZ18" s="55">
+      <c r="AZ18" s="54">
         <f t="shared" si="55"/>
         <v>4556</v>
       </c>
@@ -6574,7 +6578,7 @@
         <f t="shared" si="57"/>
         <v>4564</v>
       </c>
-      <c r="BC18" s="55">
+      <c r="BC18" s="54">
         <f t="shared" si="58"/>
         <v>4568</v>
       </c>
@@ -6679,7 +6683,7 @@
       <c r="DW18" s="1"/>
       <c r="DX18" s="1"/>
     </row>
-    <row r="19" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:128">
       <c r="A19" s="16">
         <f t="shared" si="4"/>
         <v>4608</v>
@@ -6820,7 +6824,7 @@
         <f t="shared" si="38"/>
         <v>4744</v>
       </c>
-      <c r="AJ19" s="55">
+      <c r="AJ19" s="54">
         <f t="shared" si="39"/>
         <v>4748</v>
       </c>
@@ -6832,7 +6836,7 @@
         <f t="shared" si="41"/>
         <v>4756</v>
       </c>
-      <c r="AM19" s="55">
+      <c r="AM19" s="54">
         <f t="shared" si="42"/>
         <v>4760</v>
       </c>
@@ -6844,7 +6848,7 @@
         <f t="shared" si="44"/>
         <v>4768</v>
       </c>
-      <c r="AP19" s="55">
+      <c r="AP19" s="54">
         <f t="shared" si="45"/>
         <v>4772</v>
       </c>
@@ -6860,7 +6864,7 @@
         <f t="shared" si="48"/>
         <v>4784</v>
       </c>
-      <c r="AT19" s="55">
+      <c r="AT19" s="54">
         <f t="shared" si="49"/>
         <v>4788</v>
       </c>
@@ -6884,7 +6888,7 @@
         <f t="shared" si="54"/>
         <v>4808</v>
       </c>
-      <c r="AZ19" s="55">
+      <c r="AZ19" s="54">
         <f t="shared" si="55"/>
         <v>4812</v>
       </c>
@@ -6896,7 +6900,7 @@
         <f t="shared" si="57"/>
         <v>4820</v>
       </c>
-      <c r="BC19" s="55">
+      <c r="BC19" s="54">
         <f t="shared" si="58"/>
         <v>4824</v>
       </c>
@@ -7001,7 +7005,7 @@
       <c r="DW19" s="1"/>
       <c r="DX19" s="1"/>
     </row>
-    <row r="20" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:128">
       <c r="A20" s="16">
         <f t="shared" si="4"/>
         <v>4864</v>
@@ -7142,19 +7146,19 @@
         <f t="shared" si="38"/>
         <v>5000</v>
       </c>
-      <c r="AJ20" s="55">
+      <c r="AJ20" s="54">
         <f t="shared" si="39"/>
         <v>5004</v>
       </c>
-      <c r="AK20" s="55">
+      <c r="AK20" s="54">
         <f t="shared" si="40"/>
         <v>5008</v>
       </c>
-      <c r="AL20" s="55">
+      <c r="AL20" s="54">
         <f t="shared" si="41"/>
         <v>5012</v>
       </c>
-      <c r="AM20" s="55">
+      <c r="AM20" s="54">
         <f t="shared" si="42"/>
         <v>5016</v>
       </c>
@@ -7206,7 +7210,7 @@
         <f t="shared" si="54"/>
         <v>5064</v>
       </c>
-      <c r="AZ20" s="55">
+      <c r="AZ20" s="54">
         <f t="shared" si="55"/>
         <v>5068</v>
       </c>
@@ -7218,7 +7222,7 @@
         <f t="shared" si="57"/>
         <v>5076</v>
       </c>
-      <c r="BC20" s="55">
+      <c r="BC20" s="54">
         <f t="shared" si="58"/>
         <v>5080</v>
       </c>
@@ -7323,7 +7327,7 @@
       <c r="DW20" s="1"/>
       <c r="DX20" s="1"/>
     </row>
-    <row r="21" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:128">
       <c r="A21" s="16">
         <f t="shared" si="4"/>
         <v>5120</v>
@@ -7464,7 +7468,7 @@
         <f t="shared" si="38"/>
         <v>5256</v>
       </c>
-      <c r="AJ21" s="55">
+      <c r="AJ21" s="54">
         <f t="shared" si="39"/>
         <v>5260</v>
       </c>
@@ -7488,7 +7492,7 @@
         <f t="shared" si="44"/>
         <v>5280</v>
       </c>
-      <c r="AP21" s="55">
+      <c r="AP21" s="54">
         <f t="shared" si="45"/>
         <v>5284</v>
       </c>
@@ -7504,7 +7508,7 @@
         <f t="shared" si="48"/>
         <v>5296</v>
       </c>
-      <c r="AT21" s="55">
+      <c r="AT21" s="54">
         <f t="shared" si="49"/>
         <v>5300</v>
       </c>
@@ -7528,7 +7532,7 @@
         <f t="shared" si="54"/>
         <v>5320</v>
       </c>
-      <c r="AZ21" s="55">
+      <c r="AZ21" s="54">
         <f t="shared" si="55"/>
         <v>5324</v>
       </c>
@@ -7540,7 +7544,7 @@
         <f t="shared" si="57"/>
         <v>5332</v>
       </c>
-      <c r="BC21" s="55">
+      <c r="BC21" s="54">
         <f t="shared" si="58"/>
         <v>5336</v>
       </c>
@@ -7645,7 +7649,7 @@
       <c r="DW21" s="1"/>
       <c r="DX21" s="1"/>
     </row>
-    <row r="22" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:128">
       <c r="A22" s="16">
         <f t="shared" si="4"/>
         <v>5376</v>
@@ -7786,7 +7790,7 @@
         <f t="shared" si="38"/>
         <v>5512</v>
       </c>
-      <c r="AJ22" s="55">
+      <c r="AJ22" s="54">
         <f t="shared" si="39"/>
         <v>5516</v>
       </c>
@@ -7810,7 +7814,7 @@
         <f t="shared" si="44"/>
         <v>5536</v>
       </c>
-      <c r="AP22" s="55">
+      <c r="AP22" s="54">
         <f t="shared" si="45"/>
         <v>5540</v>
       </c>
@@ -7826,7 +7830,7 @@
         <f t="shared" si="48"/>
         <v>5552</v>
       </c>
-      <c r="AT22" s="55">
+      <c r="AT22" s="54">
         <f t="shared" si="49"/>
         <v>5556</v>
       </c>
@@ -7850,7 +7854,7 @@
         <f t="shared" si="54"/>
         <v>5576</v>
       </c>
-      <c r="AZ22" s="55">
+      <c r="AZ22" s="54">
         <f t="shared" si="55"/>
         <v>5580</v>
       </c>
@@ -7862,7 +7866,7 @@
         <f t="shared" si="57"/>
         <v>5588</v>
       </c>
-      <c r="BC22" s="55">
+      <c r="BC22" s="54">
         <f t="shared" si="58"/>
         <v>5592</v>
       </c>
@@ -7967,7 +7971,7 @@
       <c r="DW22" s="1"/>
       <c r="DX22" s="1"/>
     </row>
-    <row r="23" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:128">
       <c r="A23" s="16">
         <f t="shared" si="4"/>
         <v>5632</v>
@@ -8108,7 +8112,7 @@
         <f t="shared" si="38"/>
         <v>5768</v>
       </c>
-      <c r="AJ23" s="55">
+      <c r="AJ23" s="54">
         <f t="shared" si="39"/>
         <v>5772</v>
       </c>
@@ -8124,7 +8128,7 @@
         <f t="shared" si="42"/>
         <v>5784</v>
       </c>
-      <c r="AN23" s="55">
+      <c r="AN23" s="54">
         <f t="shared" si="43"/>
         <v>5788</v>
       </c>
@@ -8132,7 +8136,7 @@
         <f t="shared" si="44"/>
         <v>5792</v>
       </c>
-      <c r="AP23" s="55">
+      <c r="AP23" s="54">
         <f t="shared" si="45"/>
         <v>5796</v>
       </c>
@@ -8148,7 +8152,7 @@
         <f t="shared" si="48"/>
         <v>5808</v>
       </c>
-      <c r="AT23" s="55">
+      <c r="AT23" s="54">
         <f t="shared" si="49"/>
         <v>5812</v>
       </c>
@@ -8172,7 +8176,7 @@
         <f t="shared" si="54"/>
         <v>5832</v>
       </c>
-      <c r="AZ23" s="55">
+      <c r="AZ23" s="54">
         <f t="shared" si="55"/>
         <v>5836</v>
       </c>
@@ -8184,7 +8188,7 @@
         <f t="shared" si="57"/>
         <v>5844</v>
       </c>
-      <c r="BC23" s="55">
+      <c r="BC23" s="54">
         <f t="shared" si="58"/>
         <v>5848</v>
       </c>
@@ -8289,7 +8293,7 @@
       <c r="DW23" s="1"/>
       <c r="DX23" s="1"/>
     </row>
-    <row r="24" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:128">
       <c r="A24" s="16">
         <f t="shared" si="4"/>
         <v>5888</v>
@@ -8430,7 +8434,7 @@
         <f t="shared" si="38"/>
         <v>6024</v>
       </c>
-      <c r="AJ24" s="55">
+      <c r="AJ24" s="54">
         <f t="shared" si="39"/>
         <v>6028</v>
       </c>
@@ -8446,7 +8450,7 @@
         <f t="shared" si="42"/>
         <v>6040</v>
       </c>
-      <c r="AN24" s="55">
+      <c r="AN24" s="54">
         <f t="shared" si="43"/>
         <v>6044</v>
       </c>
@@ -8458,15 +8462,15 @@
         <f t="shared" si="45"/>
         <v>6052</v>
       </c>
-      <c r="AQ24" s="55">
+      <c r="AQ24" s="54">
         <f t="shared" si="46"/>
         <v>6056</v>
       </c>
-      <c r="AR24" s="55">
+      <c r="AR24" s="54">
         <f t="shared" si="47"/>
         <v>6060</v>
       </c>
-      <c r="AS24" s="55">
+      <c r="AS24" s="54">
         <f t="shared" si="48"/>
         <v>6064</v>
       </c>
@@ -8498,15 +8502,15 @@
         <f t="shared" si="55"/>
         <v>6092</v>
       </c>
-      <c r="BA24" s="55">
+      <c r="BA24" s="54">
         <f t="shared" si="56"/>
         <v>6096</v>
       </c>
-      <c r="BB24" s="55">
+      <c r="BB24" s="54">
         <f t="shared" si="57"/>
         <v>6100</v>
       </c>
-      <c r="BC24" s="55">
+      <c r="BC24" s="54">
         <f t="shared" si="58"/>
         <v>6104</v>
       </c>
@@ -8611,7 +8615,7 @@
       <c r="DW24" s="1"/>
       <c r="DX24" s="1"/>
     </row>
-    <row r="25" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:128">
       <c r="A25" s="16">
         <f t="shared" si="4"/>
         <v>6144</v>
@@ -8933,7 +8937,7 @@
       <c r="DW25" s="1"/>
       <c r="DX25" s="1"/>
     </row>
-    <row r="26" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:128">
       <c r="A26" s="16">
         <f t="shared" si="4"/>
         <v>6400</v>
@@ -9255,7 +9259,7 @@
       <c r="DW26" s="1"/>
       <c r="DX26" s="1"/>
     </row>
-    <row r="27" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:128">
       <c r="A27" s="16">
         <f t="shared" si="4"/>
         <v>6656</v>
@@ -9396,7 +9400,7 @@
         <f t="shared" si="38"/>
         <v>6792</v>
       </c>
-      <c r="AJ27" s="20">
+      <c r="AJ27" s="59">
         <f t="shared" si="39"/>
         <v>6796</v>
       </c>
@@ -9404,7 +9408,7 @@
         <f t="shared" si="40"/>
         <v>6800</v>
       </c>
-      <c r="AL27" s="20">
+      <c r="AL27" s="59">
         <f t="shared" si="41"/>
         <v>6804</v>
       </c>
@@ -9420,7 +9424,7 @@
         <f t="shared" si="44"/>
         <v>6816</v>
       </c>
-      <c r="AP27" s="20">
+      <c r="AP27" s="59">
         <f t="shared" si="45"/>
         <v>6820</v>
       </c>
@@ -9428,7 +9432,7 @@
         <f t="shared" si="46"/>
         <v>6824</v>
       </c>
-      <c r="AR27" s="20">
+      <c r="AR27" s="59">
         <f t="shared" si="47"/>
         <v>6828</v>
       </c>
@@ -9444,7 +9448,7 @@
         <f t="shared" si="50"/>
         <v>6840</v>
       </c>
-      <c r="AV27" s="20">
+      <c r="AV27" s="59">
         <f t="shared" si="51"/>
         <v>6844</v>
       </c>
@@ -9452,7 +9456,7 @@
         <f t="shared" si="52"/>
         <v>6848</v>
       </c>
-      <c r="AX27" s="20">
+      <c r="AX27" s="59">
         <f t="shared" si="53"/>
         <v>6852</v>
       </c>
@@ -9577,7 +9581,7 @@
       <c r="DW27" s="1"/>
       <c r="DX27" s="1"/>
     </row>
-    <row r="28" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:128">
       <c r="A28" s="16">
         <f t="shared" si="4"/>
         <v>6912</v>
@@ -9714,23 +9718,23 @@
         <f t="shared" si="37"/>
         <v>7044</v>
       </c>
-      <c r="AI28" s="20">
+      <c r="AI28" s="59">
         <f t="shared" si="38"/>
         <v>7048</v>
       </c>
-      <c r="AJ28" s="20">
+      <c r="AJ28" s="59">
         <f t="shared" si="39"/>
         <v>7052</v>
       </c>
-      <c r="AK28" s="20">
+      <c r="AK28" s="59">
         <f t="shared" si="40"/>
         <v>7056</v>
       </c>
-      <c r="AL28" s="20">
+      <c r="AL28" s="59">
         <f t="shared" si="41"/>
         <v>7060</v>
       </c>
-      <c r="AM28" s="20">
+      <c r="AM28" s="59">
         <f t="shared" si="42"/>
         <v>7064</v>
       </c>
@@ -9738,23 +9742,23 @@
         <f t="shared" si="43"/>
         <v>7068</v>
       </c>
-      <c r="AO28" s="20">
+      <c r="AO28" s="59">
         <f t="shared" si="44"/>
         <v>7072</v>
       </c>
-      <c r="AP28" s="20">
+      <c r="AP28" s="59">
         <f t="shared" si="45"/>
         <v>7076</v>
       </c>
-      <c r="AQ28" s="20">
+      <c r="AQ28" s="59">
         <f t="shared" si="46"/>
         <v>7080</v>
       </c>
-      <c r="AR28" s="20">
+      <c r="AR28" s="59">
         <f t="shared" si="47"/>
         <v>7084</v>
       </c>
-      <c r="AS28" s="20">
+      <c r="AS28" s="59">
         <f t="shared" si="48"/>
         <v>7088</v>
       </c>
@@ -9762,23 +9766,23 @@
         <f t="shared" si="49"/>
         <v>7092</v>
       </c>
-      <c r="AU28" s="20">
+      <c r="AU28" s="59">
         <f t="shared" si="50"/>
         <v>7096</v>
       </c>
-      <c r="AV28" s="20">
+      <c r="AV28" s="59">
         <f t="shared" si="51"/>
         <v>7100</v>
       </c>
-      <c r="AW28" s="20">
+      <c r="AW28" s="59">
         <f t="shared" si="52"/>
         <v>7104</v>
       </c>
-      <c r="AX28" s="20">
+      <c r="AX28" s="59">
         <f t="shared" si="53"/>
         <v>7108</v>
       </c>
-      <c r="AY28" s="20">
+      <c r="AY28" s="59">
         <f t="shared" si="54"/>
         <v>7112</v>
       </c>
@@ -9899,7 +9903,7 @@
       <c r="DW28" s="1"/>
       <c r="DX28" s="1"/>
     </row>
-    <row r="29" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:128">
       <c r="A29" s="16">
         <f t="shared" si="4"/>
         <v>7168</v>
@@ -10036,23 +10040,23 @@
         <f t="shared" si="37"/>
         <v>7300</v>
       </c>
-      <c r="AI29" s="20">
+      <c r="AI29" s="59">
         <f t="shared" si="38"/>
         <v>7304</v>
       </c>
-      <c r="AJ29" s="20">
+      <c r="AJ29" s="59">
         <f t="shared" si="39"/>
         <v>7308</v>
       </c>
-      <c r="AK29" s="20">
+      <c r="AK29" s="59">
         <f t="shared" si="40"/>
         <v>7312</v>
       </c>
-      <c r="AL29" s="20">
+      <c r="AL29" s="59">
         <f t="shared" si="41"/>
         <v>7316</v>
       </c>
-      <c r="AM29" s="20">
+      <c r="AM29" s="59">
         <f t="shared" si="42"/>
         <v>7320</v>
       </c>
@@ -10060,23 +10064,23 @@
         <f t="shared" si="43"/>
         <v>7324</v>
       </c>
-      <c r="AO29" s="20">
+      <c r="AO29" s="59">
         <f t="shared" si="44"/>
         <v>7328</v>
       </c>
-      <c r="AP29" s="20">
+      <c r="AP29" s="59">
         <f t="shared" si="45"/>
         <v>7332</v>
       </c>
-      <c r="AQ29" s="20">
+      <c r="AQ29" s="59">
         <f t="shared" si="46"/>
         <v>7336</v>
       </c>
-      <c r="AR29" s="20">
+      <c r="AR29" s="59">
         <f t="shared" si="47"/>
         <v>7340</v>
       </c>
-      <c r="AS29" s="20">
+      <c r="AS29" s="59">
         <f t="shared" si="48"/>
         <v>7344</v>
       </c>
@@ -10084,23 +10088,23 @@
         <f t="shared" si="49"/>
         <v>7348</v>
       </c>
-      <c r="AU29" s="20">
+      <c r="AU29" s="59">
         <f t="shared" si="50"/>
         <v>7352</v>
       </c>
-      <c r="AV29" s="20">
+      <c r="AV29" s="59">
         <f t="shared" si="51"/>
         <v>7356</v>
       </c>
-      <c r="AW29" s="20">
+      <c r="AW29" s="59">
         <f t="shared" si="52"/>
         <v>7360</v>
       </c>
-      <c r="AX29" s="20">
+      <c r="AX29" s="59">
         <f t="shared" si="53"/>
         <v>7364</v>
       </c>
-      <c r="AY29" s="20">
+      <c r="AY29" s="59">
         <f t="shared" si="54"/>
         <v>7368</v>
       </c>
@@ -10221,7 +10225,7 @@
       <c r="DW29" s="1"/>
       <c r="DX29" s="1"/>
     </row>
-    <row r="30" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:128">
       <c r="A30" s="16">
         <f t="shared" si="4"/>
         <v>7424</v>
@@ -10362,15 +10366,15 @@
         <f t="shared" si="38"/>
         <v>7560</v>
       </c>
-      <c r="AJ30" s="23">
+      <c r="AJ30" s="60">
         <f t="shared" si="39"/>
         <v>7564</v>
       </c>
-      <c r="AK30" s="23">
+      <c r="AK30" s="60">
         <f t="shared" si="40"/>
         <v>7568</v>
       </c>
-      <c r="AL30" s="23">
+      <c r="AL30" s="60">
         <f t="shared" si="41"/>
         <v>7572</v>
       </c>
@@ -10386,15 +10390,15 @@
         <f t="shared" si="44"/>
         <v>7584</v>
       </c>
-      <c r="AP30" s="23">
+      <c r="AP30" s="60">
         <f t="shared" si="45"/>
         <v>7588</v>
       </c>
-      <c r="AQ30" s="23">
+      <c r="AQ30" s="60">
         <f t="shared" si="46"/>
         <v>7592</v>
       </c>
-      <c r="AR30" s="23">
+      <c r="AR30" s="60">
         <f t="shared" si="47"/>
         <v>7596</v>
       </c>
@@ -10410,15 +10414,15 @@
         <f t="shared" si="50"/>
         <v>7608</v>
       </c>
-      <c r="AV30" s="23">
+      <c r="AV30" s="60">
         <f t="shared" si="51"/>
         <v>7612</v>
       </c>
-      <c r="AW30" s="23">
+      <c r="AW30" s="60">
         <f t="shared" si="52"/>
         <v>7616</v>
       </c>
-      <c r="AX30" s="23">
+      <c r="AX30" s="60">
         <f t="shared" si="53"/>
         <v>7620</v>
       </c>
@@ -10543,7 +10547,7 @@
       <c r="DW30" s="1"/>
       <c r="DX30" s="1"/>
     </row>
-    <row r="31" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:128">
       <c r="A31" s="16">
         <f t="shared" si="4"/>
         <v>7680</v>
@@ -10688,7 +10692,7 @@
         <f t="shared" si="39"/>
         <v>7820</v>
       </c>
-      <c r="AK31" s="16">
+      <c r="AK31" s="61">
         <f t="shared" si="40"/>
         <v>7824</v>
       </c>
@@ -10712,7 +10716,7 @@
         <f t="shared" si="45"/>
         <v>7844</v>
       </c>
-      <c r="AQ31" s="16">
+      <c r="AQ31" s="61">
         <f t="shared" si="46"/>
         <v>7848</v>
       </c>
@@ -10736,7 +10740,7 @@
         <f t="shared" si="51"/>
         <v>7868</v>
       </c>
-      <c r="AW31" s="16">
+      <c r="AW31" s="61">
         <f t="shared" si="52"/>
         <v>7872</v>
       </c>
@@ -10865,7 +10869,7 @@
       <c r="DW31" s="1"/>
       <c r="DX31" s="1"/>
     </row>
-    <row r="32" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:128">
       <c r="A32" s="17">
         <f t="shared" si="4"/>
         <v>7936</v>
@@ -11187,7 +11191,7 @@
       <c r="DW32" s="1"/>
       <c r="DX32" s="1"/>
     </row>
-    <row r="33" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:128">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -11317,7 +11321,7 @@
       <c r="DW33" s="1"/>
       <c r="DX33" s="1"/>
     </row>
-    <row r="34" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:128">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -11447,7 +11451,7 @@
       <c r="DW34" s="1"/>
       <c r="DX34" s="1"/>
     </row>
-    <row r="35" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:128">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -11577,7 +11581,7 @@
       <c r="DW35" s="1"/>
       <c r="DX35" s="1"/>
     </row>
-    <row r="36" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:128">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -11707,7 +11711,7 @@
       <c r="DW36" s="1"/>
       <c r="DX36" s="1"/>
     </row>
-    <row r="37" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:128">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -11837,7 +11841,7 @@
       <c r="DW37" s="1"/>
       <c r="DX37" s="1"/>
     </row>
-    <row r="38" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:128">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -11967,7 +11971,7 @@
       <c r="DW38" s="1"/>
       <c r="DX38" s="1"/>
     </row>
-    <row r="39" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:128">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -12097,7 +12101,7 @@
       <c r="DW39" s="1"/>
       <c r="DX39" s="1"/>
     </row>
-    <row r="40" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:128">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -12227,7 +12231,7 @@
       <c r="DW40" s="1"/>
       <c r="DX40" s="1"/>
     </row>
-    <row r="41" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:128">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -12357,7 +12361,7 @@
       <c r="DW41" s="1"/>
       <c r="DX41" s="1"/>
     </row>
-    <row r="42" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:128">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -12487,7 +12491,7 @@
       <c r="DW42" s="1"/>
       <c r="DX42" s="1"/>
     </row>
-    <row r="43" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:128">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -12617,7 +12621,7 @@
       <c r="DW43" s="1"/>
       <c r="DX43" s="1"/>
     </row>
-    <row r="44" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:128">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -12747,7 +12751,7 @@
       <c r="DW44" s="1"/>
       <c r="DX44" s="1"/>
     </row>
-    <row r="45" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:128">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -12877,7 +12881,7 @@
       <c r="DW45" s="1"/>
       <c r="DX45" s="1"/>
     </row>
-    <row r="46" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:128">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -13007,7 +13011,7 @@
       <c r="DW46" s="1"/>
       <c r="DX46" s="1"/>
     </row>
-    <row r="47" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:128">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -13137,7 +13141,7 @@
       <c r="DW47" s="1"/>
       <c r="DX47" s="1"/>
     </row>
-    <row r="48" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:128">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -13267,7 +13271,7 @@
       <c r="DW48" s="1"/>
       <c r="DX48" s="1"/>
     </row>
-    <row r="49" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:128">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -13397,7 +13401,7 @@
       <c r="DW49" s="1"/>
       <c r="DX49" s="1"/>
     </row>
-    <row r="50" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:128">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -13527,7 +13531,7 @@
       <c r="DW50" s="1"/>
       <c r="DX50" s="1"/>
     </row>
-    <row r="51" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:128">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -13657,7 +13661,7 @@
       <c r="DW51" s="1"/>
       <c r="DX51" s="1"/>
     </row>
-    <row r="52" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:128">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -13787,7 +13791,7 @@
       <c r="DW52" s="1"/>
       <c r="DX52" s="1"/>
     </row>
-    <row r="53" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:128">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -13917,7 +13921,7 @@
       <c r="DW53" s="1"/>
       <c r="DX53" s="1"/>
     </row>
-    <row r="54" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:128">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -14047,7 +14051,7 @@
       <c r="DW54" s="1"/>
       <c r="DX54" s="1"/>
     </row>
-    <row r="55" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:128">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -14177,7 +14181,7 @@
       <c r="DW55" s="1"/>
       <c r="DX55" s="1"/>
     </row>
-    <row r="56" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:128">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -14307,7 +14311,7 @@
       <c r="DW56" s="1"/>
       <c r="DX56" s="1"/>
     </row>
-    <row r="57" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:128">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -14437,7 +14441,7 @@
       <c r="DW57" s="1"/>
       <c r="DX57" s="1"/>
     </row>
-    <row r="58" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:128">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -14567,7 +14571,7 @@
       <c r="DW58" s="1"/>
       <c r="DX58" s="1"/>
     </row>
-    <row r="59" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:128">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -14697,7 +14701,7 @@
       <c r="DW59" s="1"/>
       <c r="DX59" s="1"/>
     </row>
-    <row r="60" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:128">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -14827,7 +14831,7 @@
       <c r="DW60" s="1"/>
       <c r="DX60" s="1"/>
     </row>
-    <row r="61" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:128">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -14957,7 +14961,7 @@
       <c r="DW61" s="1"/>
       <c r="DX61" s="1"/>
     </row>
-    <row r="62" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:128">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -15087,7 +15091,7 @@
       <c r="DW62" s="1"/>
       <c r="DX62" s="1"/>
     </row>
-    <row r="63" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:128">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -15217,7 +15221,7 @@
       <c r="DW63" s="1"/>
       <c r="DX63" s="1"/>
     </row>
-    <row r="64" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:128">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -15354,14 +15358,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BL32"/>
   <sheetViews>
     <sheetView topLeftCell="A8" zoomScale="82" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="AJ14" sqref="AJ14:AO24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.140625" customWidth="1"/>
     <col min="2" max="2" width="5.7109375" customWidth="1"/>
@@ -15392,7 +15396,7 @@
     <col min="31" max="31" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:64">
       <c r="A1" s="18">
         <v>0</v>
       </c>
@@ -15649,7 +15653,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="2" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:64">
       <c r="A2" s="18">
         <f t="shared" ref="A2:AE10" si="2">A1+256</f>
         <v>256</v>
@@ -15907,7 +15911,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:64">
       <c r="A3" s="18">
         <f t="shared" si="2"/>
         <v>512</v>
@@ -16165,7 +16169,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:64">
       <c r="A4" s="18">
         <f t="shared" si="2"/>
         <v>768</v>
@@ -16423,7 +16427,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:64">
       <c r="A5" s="18">
         <f t="shared" si="2"/>
         <v>1024</v>
@@ -16681,7 +16685,7 @@
         <v>1276</v>
       </c>
     </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:64">
       <c r="A6" s="18">
         <f t="shared" si="2"/>
         <v>1280</v>
@@ -16939,7 +16943,7 @@
         <v>1532</v>
       </c>
     </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:64">
       <c r="A7" s="18">
         <f t="shared" si="2"/>
         <v>1536</v>
@@ -17197,7 +17201,7 @@
         <v>1788</v>
       </c>
     </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:64">
       <c r="A8" s="18">
         <f t="shared" si="2"/>
         <v>1792</v>
@@ -17455,7 +17459,7 @@
         <v>2044</v>
       </c>
     </row>
-    <row r="9" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:64">
       <c r="A9" s="18">
         <f t="shared" si="2"/>
         <v>2048</v>
@@ -17713,7 +17717,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:64">
       <c r="A10" s="18">
         <f t="shared" si="2"/>
         <v>2304</v>
@@ -17971,7 +17975,7 @@
         <v>2556</v>
       </c>
     </row>
-    <row r="11" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:64">
       <c r="A11" s="18">
         <f t="shared" ref="A11:P26" si="8">A10+256</f>
         <v>2560</v>
@@ -18229,7 +18233,7 @@
         <v>2812</v>
       </c>
     </row>
-    <row r="12" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:64">
       <c r="A12" s="18">
         <f t="shared" si="8"/>
         <v>2816</v>
@@ -18487,7 +18491,7 @@
         <v>3068</v>
       </c>
     </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:64">
       <c r="A13" s="18">
         <f t="shared" si="8"/>
         <v>3072</v>
@@ -18745,7 +18749,7 @@
         <v>3324</v>
       </c>
     </row>
-    <row r="14" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:64">
       <c r="A14" s="18">
         <f t="shared" si="8"/>
         <v>3328</v>
@@ -18890,19 +18894,19 @@
         <f t="shared" si="4"/>
         <v>3468</v>
       </c>
-      <c r="AK14" s="57">
+      <c r="AK14" s="56">
         <f t="shared" si="4"/>
         <v>3472</v>
       </c>
-      <c r="AL14" s="57">
+      <c r="AL14" s="56">
         <f t="shared" si="4"/>
         <v>3476</v>
       </c>
-      <c r="AM14" s="57">
+      <c r="AM14" s="56">
         <f t="shared" si="4"/>
         <v>3480</v>
       </c>
-      <c r="AN14" s="57">
+      <c r="AN14" s="56">
         <f t="shared" si="4"/>
         <v>3484</v>
       </c>
@@ -18914,19 +18918,19 @@
         <f t="shared" si="4"/>
         <v>3492</v>
       </c>
-      <c r="AQ14" s="57">
+      <c r="AQ14" s="56">
         <f t="shared" si="4"/>
         <v>3496</v>
       </c>
-      <c r="AR14" s="57">
+      <c r="AR14" s="56">
         <f t="shared" si="4"/>
         <v>3500</v>
       </c>
-      <c r="AS14" s="57">
+      <c r="AS14" s="56">
         <f t="shared" si="4"/>
         <v>3504</v>
       </c>
-      <c r="AT14" s="57">
+      <c r="AT14" s="56">
         <f t="shared" si="4"/>
         <v>3508</v>
       </c>
@@ -19003,7 +19007,7 @@
         <v>3580</v>
       </c>
     </row>
-    <row r="15" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:64">
       <c r="A15" s="18">
         <f t="shared" si="8"/>
         <v>3584</v>
@@ -19144,7 +19148,7 @@
         <f t="shared" si="4"/>
         <v>3720</v>
       </c>
-      <c r="AJ15" s="57">
+      <c r="AJ15" s="56">
         <f t="shared" si="4"/>
         <v>3724</v>
       </c>
@@ -19164,7 +19168,7 @@
         <f t="shared" si="4"/>
         <v>3740</v>
       </c>
-      <c r="AO15" s="57">
+      <c r="AO15" s="56">
         <f t="shared" si="4"/>
         <v>3744</v>
       </c>
@@ -19188,7 +19192,7 @@
         <f t="shared" si="4"/>
         <v>3764</v>
       </c>
-      <c r="AU15" s="57">
+      <c r="AU15" s="56">
         <f t="shared" si="4"/>
         <v>3768</v>
       </c>
@@ -19261,7 +19265,7 @@
         <v>3836</v>
       </c>
     </row>
-    <row r="16" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:64">
       <c r="A16" s="18">
         <f t="shared" si="8"/>
         <v>3840</v>
@@ -19402,7 +19406,7 @@
         <f t="shared" si="4"/>
         <v>3976</v>
       </c>
-      <c r="AJ16" s="57">
+      <c r="AJ16" s="56">
         <f t="shared" si="4"/>
         <v>3980</v>
       </c>
@@ -19422,7 +19426,7 @@
         <f t="shared" si="4"/>
         <v>3996</v>
       </c>
-      <c r="AO16" s="57">
+      <c r="AO16" s="56">
         <f t="shared" si="4"/>
         <v>4000</v>
       </c>
@@ -19446,7 +19450,7 @@
         <f t="shared" si="4"/>
         <v>4020</v>
       </c>
-      <c r="AU16" s="57">
+      <c r="AU16" s="56">
         <f t="shared" si="4"/>
         <v>4024</v>
       </c>
@@ -19519,7 +19523,7 @@
         <v>4092</v>
       </c>
     </row>
-    <row r="17" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:64">
       <c r="A17" s="18">
         <f t="shared" si="8"/>
         <v>4096</v>
@@ -19660,7 +19664,7 @@
         <f t="shared" si="4"/>
         <v>4232</v>
       </c>
-      <c r="AJ17" s="57">
+      <c r="AJ17" s="56">
         <f t="shared" si="4"/>
         <v>4236</v>
       </c>
@@ -19680,7 +19684,7 @@
         <f t="shared" si="4"/>
         <v>4252</v>
       </c>
-      <c r="AO17" s="57">
+      <c r="AO17" s="56">
         <f t="shared" si="4"/>
         <v>4256</v>
       </c>
@@ -19704,7 +19708,7 @@
         <f t="shared" si="4"/>
         <v>4276</v>
       </c>
-      <c r="AU17" s="57">
+      <c r="AU17" s="56">
         <f t="shared" si="4"/>
         <v>4280</v>
       </c>
@@ -19777,7 +19781,7 @@
         <v>4348</v>
       </c>
     </row>
-    <row r="18" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:64">
       <c r="A18" s="18">
         <f t="shared" si="8"/>
         <v>4352</v>
@@ -19918,7 +19922,7 @@
         <f t="shared" si="4"/>
         <v>4488</v>
       </c>
-      <c r="AJ18" s="57">
+      <c r="AJ18" s="56">
         <f t="shared" si="4"/>
         <v>4492</v>
       </c>
@@ -19938,7 +19942,7 @@
         <f t="shared" si="4"/>
         <v>4508</v>
       </c>
-      <c r="AO18" s="57">
+      <c r="AO18" s="56">
         <f t="shared" si="4"/>
         <v>4512</v>
       </c>
@@ -19962,7 +19966,7 @@
         <f t="shared" si="4"/>
         <v>4532</v>
       </c>
-      <c r="AU18" s="57">
+      <c r="AU18" s="56">
         <f t="shared" si="4"/>
         <v>4536</v>
       </c>
@@ -20035,7 +20039,7 @@
         <v>4604</v>
       </c>
     </row>
-    <row r="19" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:64">
       <c r="A19" s="18">
         <f t="shared" si="8"/>
         <v>4608</v>
@@ -20180,19 +20184,19 @@
         <f t="shared" si="9"/>
         <v>4748</v>
       </c>
-      <c r="AK19" s="57">
+      <c r="AK19" s="56">
         <f t="shared" si="9"/>
         <v>4752</v>
       </c>
-      <c r="AL19" s="57">
+      <c r="AL19" s="56">
         <f t="shared" si="9"/>
         <v>4756</v>
       </c>
-      <c r="AM19" s="57">
+      <c r="AM19" s="56">
         <f t="shared" si="9"/>
         <v>4760</v>
       </c>
-      <c r="AN19" s="57">
+      <c r="AN19" s="56">
         <f t="shared" si="9"/>
         <v>4764</v>
       </c>
@@ -20204,19 +20208,19 @@
         <f t="shared" si="9"/>
         <v>4772</v>
       </c>
-      <c r="AQ19" s="57">
+      <c r="AQ19" s="56">
         <f t="shared" si="9"/>
         <v>4776</v>
       </c>
-      <c r="AR19" s="57">
+      <c r="AR19" s="56">
         <f t="shared" si="9"/>
         <v>4780</v>
       </c>
-      <c r="AS19" s="57">
+      <c r="AS19" s="56">
         <f t="shared" si="9"/>
         <v>4784</v>
       </c>
-      <c r="AT19" s="57">
+      <c r="AT19" s="56">
         <f t="shared" si="9"/>
         <v>4788</v>
       </c>
@@ -20293,7 +20297,7 @@
         <v>4860</v>
       </c>
     </row>
-    <row r="20" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:64">
       <c r="A20" s="18">
         <f t="shared" si="8"/>
         <v>4864</v>
@@ -20434,7 +20438,7 @@
         <f t="shared" si="9"/>
         <v>5000</v>
       </c>
-      <c r="AJ20" s="57">
+      <c r="AJ20" s="56">
         <f t="shared" si="9"/>
         <v>5004</v>
       </c>
@@ -20454,7 +20458,7 @@
         <f t="shared" si="9"/>
         <v>5020</v>
       </c>
-      <c r="AO20" s="57">
+      <c r="AO20" s="56">
         <f t="shared" si="9"/>
         <v>5024</v>
       </c>
@@ -20478,7 +20482,7 @@
         <f t="shared" si="9"/>
         <v>5044</v>
       </c>
-      <c r="AU20" s="57">
+      <c r="AU20" s="56">
         <f t="shared" si="9"/>
         <v>5048</v>
       </c>
@@ -20551,7 +20555,7 @@
         <v>5116</v>
       </c>
     </row>
-    <row r="21" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:64">
       <c r="A21" s="18">
         <f t="shared" si="8"/>
         <v>5120</v>
@@ -20692,7 +20696,7 @@
         <f t="shared" si="9"/>
         <v>5256</v>
       </c>
-      <c r="AJ21" s="57">
+      <c r="AJ21" s="56">
         <f t="shared" si="9"/>
         <v>5260</v>
       </c>
@@ -20712,7 +20716,7 @@
         <f t="shared" si="9"/>
         <v>5276</v>
       </c>
-      <c r="AO21" s="57">
+      <c r="AO21" s="56">
         <f t="shared" si="9"/>
         <v>5280</v>
       </c>
@@ -20736,7 +20740,7 @@
         <f t="shared" si="9"/>
         <v>5300</v>
       </c>
-      <c r="AU21" s="57">
+      <c r="AU21" s="56">
         <f t="shared" si="9"/>
         <v>5304</v>
       </c>
@@ -20809,7 +20813,7 @@
         <v>5372</v>
       </c>
     </row>
-    <row r="22" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:64">
       <c r="A22" s="18">
         <f t="shared" si="8"/>
         <v>5376</v>
@@ -20950,7 +20954,7 @@
         <f t="shared" si="9"/>
         <v>5512</v>
       </c>
-      <c r="AJ22" s="57">
+      <c r="AJ22" s="56">
         <f t="shared" si="9"/>
         <v>5516</v>
       </c>
@@ -20970,7 +20974,7 @@
         <f t="shared" si="9"/>
         <v>5532</v>
       </c>
-      <c r="AO22" s="57">
+      <c r="AO22" s="56">
         <f t="shared" si="9"/>
         <v>5536</v>
       </c>
@@ -20994,7 +20998,7 @@
         <f t="shared" si="9"/>
         <v>5556</v>
       </c>
-      <c r="AU22" s="57">
+      <c r="AU22" s="56">
         <f t="shared" si="9"/>
         <v>5560</v>
       </c>
@@ -21067,7 +21071,7 @@
         <v>5628</v>
       </c>
     </row>
-    <row r="23" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:64">
       <c r="A23" s="18">
         <f t="shared" si="8"/>
         <v>5632</v>
@@ -21208,7 +21212,7 @@
         <f t="shared" si="9"/>
         <v>5768</v>
       </c>
-      <c r="AJ23" s="57">
+      <c r="AJ23" s="56">
         <f t="shared" si="9"/>
         <v>5772</v>
       </c>
@@ -21228,7 +21232,7 @@
         <f t="shared" si="9"/>
         <v>5788</v>
       </c>
-      <c r="AO23" s="57">
+      <c r="AO23" s="56">
         <f t="shared" si="9"/>
         <v>5792</v>
       </c>
@@ -21252,7 +21256,7 @@
         <f t="shared" si="9"/>
         <v>5812</v>
       </c>
-      <c r="AU23" s="57">
+      <c r="AU23" s="56">
         <f t="shared" si="9"/>
         <v>5816</v>
       </c>
@@ -21325,7 +21329,7 @@
         <v>5884</v>
       </c>
     </row>
-    <row r="24" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:64">
       <c r="A24" s="18">
         <f t="shared" si="8"/>
         <v>5888</v>
@@ -21470,19 +21474,19 @@
         <f t="shared" si="9"/>
         <v>6028</v>
       </c>
-      <c r="AK24" s="57">
+      <c r="AK24" s="56">
         <f t="shared" si="9"/>
         <v>6032</v>
       </c>
-      <c r="AL24" s="57">
+      <c r="AL24" s="56">
         <f t="shared" si="9"/>
         <v>6036</v>
       </c>
-      <c r="AM24" s="57">
+      <c r="AM24" s="56">
         <f t="shared" si="9"/>
         <v>6040</v>
       </c>
-      <c r="AN24" s="57">
+      <c r="AN24" s="56">
         <f t="shared" si="9"/>
         <v>6044</v>
       </c>
@@ -21494,19 +21498,19 @@
         <f t="shared" si="9"/>
         <v>6052</v>
       </c>
-      <c r="AQ24" s="57">
+      <c r="AQ24" s="56">
         <f t="shared" si="9"/>
         <v>6056</v>
       </c>
-      <c r="AR24" s="57">
+      <c r="AR24" s="56">
         <f t="shared" si="9"/>
         <v>6060</v>
       </c>
-      <c r="AS24" s="57">
+      <c r="AS24" s="56">
         <f t="shared" si="9"/>
         <v>6064</v>
       </c>
-      <c r="AT24" s="57">
+      <c r="AT24" s="56">
         <f t="shared" si="9"/>
         <v>6068</v>
       </c>
@@ -21583,7 +21587,7 @@
         <v>6140</v>
       </c>
     </row>
-    <row r="25" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:64">
       <c r="A25" s="18">
         <f t="shared" si="8"/>
         <v>6144</v>
@@ -21841,7 +21845,7 @@
         <v>6396</v>
       </c>
     </row>
-    <row r="26" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:64">
       <c r="A26" s="18">
         <f t="shared" si="8"/>
         <v>6400</v>
@@ -22099,7 +22103,7 @@
         <v>6652</v>
       </c>
     </row>
-    <row r="27" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:64">
       <c r="A27" s="18">
         <f t="shared" ref="A27:P32" si="14">A26+256</f>
         <v>6656</v>
@@ -22357,7 +22361,7 @@
         <v>6908</v>
       </c>
     </row>
-    <row r="28" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:64">
       <c r="A28" s="18">
         <f t="shared" si="14"/>
         <v>6912</v>
@@ -22615,7 +22619,7 @@
         <v>7164</v>
       </c>
     </row>
-    <row r="29" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:64">
       <c r="A29" s="18">
         <f t="shared" si="14"/>
         <v>7168</v>
@@ -22873,7 +22877,7 @@
         <v>7420</v>
       </c>
     </row>
-    <row r="30" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:64">
       <c r="A30" s="18">
         <f t="shared" si="14"/>
         <v>7424</v>
@@ -23131,7 +23135,7 @@
         <v>7676</v>
       </c>
     </row>
-    <row r="31" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:64">
       <c r="A31" s="18">
         <f t="shared" si="14"/>
         <v>7680</v>
@@ -23389,7 +23393,7 @@
         <v>7932</v>
       </c>
     </row>
-    <row r="32" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:64">
       <c r="A32" s="18">
         <f t="shared" si="14"/>
         <v>7936</v>
@@ -23654,16 +23658,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BL32"/>
   <sheetViews>
     <sheetView topLeftCell="R1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:64">
       <c r="A1" s="5">
         <v>0</v>
       </c>
@@ -23920,7 +23924,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="2" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:64">
       <c r="A2" s="5">
         <f t="shared" ref="A2:AE10" si="2">A1+256</f>
         <v>256</v>
@@ -24178,7 +24182,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:64">
       <c r="A3" s="5">
         <f t="shared" si="2"/>
         <v>512</v>
@@ -24436,7 +24440,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:64">
       <c r="A4" s="5">
         <f t="shared" si="2"/>
         <v>768</v>
@@ -24694,7 +24698,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:64">
       <c r="A5" s="5">
         <f t="shared" si="2"/>
         <v>1024</v>
@@ -24952,7 +24956,7 @@
         <v>1276</v>
       </c>
     </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:64">
       <c r="A6" s="5">
         <f t="shared" si="2"/>
         <v>1280</v>
@@ -25210,7 +25214,7 @@
         <v>1532</v>
       </c>
     </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:64">
       <c r="A7" s="5">
         <f t="shared" si="2"/>
         <v>1536</v>
@@ -25468,7 +25472,7 @@
         <v>1788</v>
       </c>
     </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:64">
       <c r="A8" s="5">
         <f t="shared" si="2"/>
         <v>1792</v>
@@ -25726,7 +25730,7 @@
         <v>2044</v>
       </c>
     </row>
-    <row r="9" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:64">
       <c r="A9" s="5">
         <f t="shared" si="2"/>
         <v>2048</v>
@@ -25984,7 +25988,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:64">
       <c r="A10" s="5">
         <f t="shared" si="2"/>
         <v>2304</v>
@@ -26242,7 +26246,7 @@
         <v>2556</v>
       </c>
     </row>
-    <row r="11" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:64">
       <c r="A11" s="5">
         <f t="shared" ref="A11:P26" si="8">A10+256</f>
         <v>2560</v>
@@ -26500,7 +26504,7 @@
         <v>2812</v>
       </c>
     </row>
-    <row r="12" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:64">
       <c r="A12" s="5">
         <f t="shared" si="8"/>
         <v>2816</v>
@@ -26758,7 +26762,7 @@
         <v>3068</v>
       </c>
     </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:64">
       <c r="A13" s="5">
         <f t="shared" si="8"/>
         <v>3072</v>
@@ -27016,7 +27020,7 @@
         <v>3324</v>
       </c>
     </row>
-    <row r="14" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:64">
       <c r="A14" s="5">
         <f t="shared" si="8"/>
         <v>3328</v>
@@ -27274,7 +27278,7 @@
         <v>3580</v>
       </c>
     </row>
-    <row r="15" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:64">
       <c r="A15" s="5">
         <f t="shared" si="8"/>
         <v>3584</v>
@@ -27532,7 +27536,7 @@
         <v>3836</v>
       </c>
     </row>
-    <row r="16" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:64">
       <c r="A16" s="5">
         <f t="shared" si="8"/>
         <v>3840</v>
@@ -27790,7 +27794,7 @@
         <v>4092</v>
       </c>
     </row>
-    <row r="17" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:64">
       <c r="A17" s="5">
         <f t="shared" si="8"/>
         <v>4096</v>
@@ -28048,7 +28052,7 @@
         <v>4348</v>
       </c>
     </row>
-    <row r="18" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:64">
       <c r="A18" s="5">
         <f t="shared" si="8"/>
         <v>4352</v>
@@ -28306,7 +28310,7 @@
         <v>4604</v>
       </c>
     </row>
-    <row r="19" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:64">
       <c r="A19" s="5">
         <f t="shared" si="8"/>
         <v>4608</v>
@@ -28564,7 +28568,7 @@
         <v>4860</v>
       </c>
     </row>
-    <row r="20" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:64">
       <c r="A20" s="5">
         <f t="shared" si="8"/>
         <v>4864</v>
@@ -28822,7 +28826,7 @@
         <v>5116</v>
       </c>
     </row>
-    <row r="21" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:64">
       <c r="A21" s="5">
         <f t="shared" si="8"/>
         <v>5120</v>
@@ -29080,7 +29084,7 @@
         <v>5372</v>
       </c>
     </row>
-    <row r="22" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:64">
       <c r="A22" s="1">
         <f t="shared" si="8"/>
         <v>5376</v>
@@ -29338,7 +29342,7 @@
         <v>5628</v>
       </c>
     </row>
-    <row r="23" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:64">
       <c r="A23" s="1">
         <f t="shared" si="8"/>
         <v>5632</v>
@@ -29596,7 +29600,7 @@
         <v>5884</v>
       </c>
     </row>
-    <row r="24" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:64">
       <c r="A24" s="1">
         <f t="shared" si="8"/>
         <v>5888</v>
@@ -29854,7 +29858,7 @@
         <v>6140</v>
       </c>
     </row>
-    <row r="25" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:64">
       <c r="A25" s="1">
         <f t="shared" si="8"/>
         <v>6144</v>
@@ -30112,7 +30116,7 @@
         <v>6396</v>
       </c>
     </row>
-    <row r="26" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:64">
       <c r="A26" s="1">
         <f t="shared" si="8"/>
         <v>6400</v>
@@ -30370,7 +30374,7 @@
         <v>6652</v>
       </c>
     </row>
-    <row r="27" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:64">
       <c r="A27" s="1">
         <f t="shared" ref="A27:P32" si="14">A26+256</f>
         <v>6656</v>
@@ -30628,7 +30632,7 @@
         <v>6908</v>
       </c>
     </row>
-    <row r="28" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:64">
       <c r="A28" s="1">
         <f t="shared" si="14"/>
         <v>6912</v>
@@ -30886,7 +30890,7 @@
         <v>7164</v>
       </c>
     </row>
-    <row r="29" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:64">
       <c r="A29" s="1">
         <f t="shared" si="14"/>
         <v>7168</v>
@@ -31144,7 +31148,7 @@
         <v>7420</v>
       </c>
     </row>
-    <row r="30" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:64">
       <c r="A30" s="1">
         <f t="shared" si="14"/>
         <v>7424</v>
@@ -31402,7 +31406,7 @@
         <v>7676</v>
       </c>
     </row>
-    <row r="31" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:64">
       <c r="A31" s="1">
         <f t="shared" si="14"/>
         <v>7680</v>
@@ -31660,7 +31664,7 @@
         <v>7932</v>
       </c>
     </row>
-    <row r="32" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:64">
       <c r="A32" s="2">
         <f t="shared" si="14"/>
         <v>7936</v>
@@ -31924,16 +31928,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BL32"/>
   <sheetViews>
     <sheetView zoomScale="72" zoomScaleNormal="72" zoomScaleSheetLayoutView="50" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:64">
       <c r="A1" s="5">
         <v>0</v>
       </c>
@@ -32190,7 +32194,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="2" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:64">
       <c r="A2" s="5">
         <f t="shared" ref="A2:AE10" si="2">A1+256</f>
         <v>256</v>
@@ -32448,7 +32452,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:64">
       <c r="A3" s="5">
         <f t="shared" si="2"/>
         <v>512</v>
@@ -32706,7 +32710,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:64">
       <c r="A4" s="5">
         <f t="shared" si="2"/>
         <v>768</v>
@@ -32964,7 +32968,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:64">
       <c r="A5" s="5">
         <f t="shared" si="2"/>
         <v>1024</v>
@@ -33222,7 +33226,7 @@
         <v>1276</v>
       </c>
     </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:64">
       <c r="A6" s="5">
         <f t="shared" si="2"/>
         <v>1280</v>
@@ -33480,7 +33484,7 @@
         <v>1532</v>
       </c>
     </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:64">
       <c r="A7" s="5">
         <f t="shared" si="2"/>
         <v>1536</v>
@@ -33738,7 +33742,7 @@
         <v>1788</v>
       </c>
     </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:64">
       <c r="A8" s="5">
         <f t="shared" si="2"/>
         <v>1792</v>
@@ -33996,7 +34000,7 @@
         <v>2044</v>
       </c>
     </row>
-    <row r="9" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:64">
       <c r="A9" s="5">
         <f t="shared" si="2"/>
         <v>2048</v>
@@ -34254,7 +34258,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:64">
       <c r="A10" s="5">
         <f t="shared" si="2"/>
         <v>2304</v>
@@ -34512,7 +34516,7 @@
         <v>2556</v>
       </c>
     </row>
-    <row r="11" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:64">
       <c r="A11" s="5">
         <f t="shared" ref="A11:P26" si="8">A10+256</f>
         <v>2560</v>
@@ -34770,7 +34774,7 @@
         <v>2812</v>
       </c>
     </row>
-    <row r="12" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:64">
       <c r="A12" s="5">
         <f t="shared" si="8"/>
         <v>2816</v>
@@ -35028,7 +35032,7 @@
         <v>3068</v>
       </c>
     </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:64">
       <c r="A13" s="5">
         <f t="shared" si="8"/>
         <v>3072</v>
@@ -35286,7 +35290,7 @@
         <v>3324</v>
       </c>
     </row>
-    <row r="14" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:64">
       <c r="A14" s="5">
         <f t="shared" si="8"/>
         <v>3328</v>
@@ -35544,7 +35548,7 @@
         <v>3580</v>
       </c>
     </row>
-    <row r="15" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:64">
       <c r="A15" s="5">
         <f t="shared" si="8"/>
         <v>3584</v>
@@ -35802,7 +35806,7 @@
         <v>3836</v>
       </c>
     </row>
-    <row r="16" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:64">
       <c r="A16" s="5">
         <f t="shared" si="8"/>
         <v>3840</v>
@@ -36060,7 +36064,7 @@
         <v>4092</v>
       </c>
     </row>
-    <row r="17" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:64">
       <c r="A17" s="5">
         <f t="shared" si="8"/>
         <v>4096</v>
@@ -36318,7 +36322,7 @@
         <v>4348</v>
       </c>
     </row>
-    <row r="18" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:64">
       <c r="A18" s="5">
         <f t="shared" si="8"/>
         <v>4352</v>
@@ -36576,7 +36580,7 @@
         <v>4604</v>
       </c>
     </row>
-    <row r="19" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:64">
       <c r="A19" s="5">
         <f t="shared" si="8"/>
         <v>4608</v>
@@ -36834,7 +36838,7 @@
         <v>4860</v>
       </c>
     </row>
-    <row r="20" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:64">
       <c r="A20" s="5">
         <f t="shared" si="8"/>
         <v>4864</v>
@@ -37092,7 +37096,7 @@
         <v>5116</v>
       </c>
     </row>
-    <row r="21" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:64">
       <c r="A21" s="5">
         <f t="shared" si="8"/>
         <v>5120</v>
@@ -37350,7 +37354,7 @@
         <v>5372</v>
       </c>
     </row>
-    <row r="22" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:64">
       <c r="A22" s="5">
         <f t="shared" si="8"/>
         <v>5376</v>
@@ -37608,7 +37612,7 @@
         <v>5628</v>
       </c>
     </row>
-    <row r="23" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:64">
       <c r="A23" s="5">
         <f t="shared" si="8"/>
         <v>5632</v>
@@ -37866,7 +37870,7 @@
         <v>5884</v>
       </c>
     </row>
-    <row r="24" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:64">
       <c r="A24" s="5">
         <f t="shared" si="8"/>
         <v>5888</v>
@@ -38124,7 +38128,7 @@
         <v>6140</v>
       </c>
     </row>
-    <row r="25" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:64">
       <c r="A25" s="5">
         <f t="shared" si="8"/>
         <v>6144</v>
@@ -38382,7 +38386,7 @@
         <v>6396</v>
       </c>
     </row>
-    <row r="26" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:64">
       <c r="A26" s="5">
         <f t="shared" si="8"/>
         <v>6400</v>
@@ -38640,7 +38644,7 @@
         <v>6652</v>
       </c>
     </row>
-    <row r="27" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:64">
       <c r="A27" s="5">
         <f t="shared" ref="A27:P32" si="14">A26+256</f>
         <v>6656</v>
@@ -38898,7 +38902,7 @@
         <v>6908</v>
       </c>
     </row>
-    <row r="28" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:64">
       <c r="A28" s="5">
         <f t="shared" si="14"/>
         <v>6912</v>
@@ -39156,7 +39160,7 @@
         <v>7164</v>
       </c>
     </row>
-    <row r="29" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:64">
       <c r="A29" s="5">
         <f t="shared" si="14"/>
         <v>7168</v>
@@ -39414,7 +39418,7 @@
         <v>7420</v>
       </c>
     </row>
-    <row r="30" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:64">
       <c r="A30" s="5">
         <f t="shared" si="14"/>
         <v>7424</v>
@@ -39672,7 +39676,7 @@
         <v>7676</v>
       </c>
     </row>
-    <row r="31" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:64">
       <c r="A31" s="5">
         <f t="shared" si="14"/>
         <v>7680</v>
@@ -39930,7 +39934,7 @@
         <v>7932</v>
       </c>
     </row>
-    <row r="32" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:64">
       <c r="A32" s="12">
         <f t="shared" si="14"/>
         <v>7936</v>

</xml_diff>